<commit_message>
create new project finish v.1
create new project finish v.1
</commit_message>
<xml_diff>
--- a/NOTE.xlsx
+++ b/NOTE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\LEARNING\VUEJS\1\vue3_learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\LEARNING\VUEJS\Vue3EShopSolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067C34FC-EBDB-4D4A-A36B-A8BEE900DF6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D34E231-4EC9-44D0-BFD9-59EA73122D64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Set-ExecutionPolicy -Scope Process -ExecutionPolicy Bypass</t>
   </si>
@@ -54,20 +54,86 @@
     <t>Tao mới 1 app VUE</t>
   </si>
   <si>
-    <t>json-server --watch db.json</t>
-  </si>
-  <si>
     <t xml:space="preserve">      server data ảo</t>
   </si>
   <si>
     <t>lệnh trên để chạy server  (xem hình bên dưới)</t>
+  </si>
+  <si>
+    <t>Tham khao bai` học trên youtube</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=RTpx9Wykyac&amp;t=3s&amp;ab_channel=HenryWebDevHenryWebDev</t>
+  </si>
+  <si>
+    <t>copy : Set-ExecutionPolicy -Scope Process -ExecutionPolicy Bypass</t>
+  </si>
+  <si>
+    <t>json-server --watch data/db.json</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>G:\LEARNING\NODEJS\Video\0000032_08.NodeJS [5.1GB] API Masterclass With Express &amp; MongoDB\10. API Security\3. XSS Protection  Security Headers.mp4</t>
+  </si>
+  <si>
+    <t>1. Logout To Clear Token Cookie.mp4</t>
+  </si>
+  <si>
+    <t>2. Prevent NoSQL Injection  Sanitize Data.mp4</t>
+  </si>
+  <si>
+    <t>3. XSS Protection  Security Headers.mp4</t>
+  </si>
+  <si>
+    <t>4. Rate Limiting, HPP  CORS.mp4</t>
+  </si>
+  <si>
+    <t>\0000060_13.Vue JS_[6.78 GB] - Essentials with Vuex and Vue Router\3. Writing Effective Vue Apps\</t>
+  </si>
+  <si>
+    <t>https://cdnjs.com/libraries/jquery</t>
+  </si>
+  <si>
+    <t>    &lt;script src="https://cdnjs.cloudflare.com/ajax/libs/jquery/3.6.0/jquery.min.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;link rel="stylesheet" href="https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/css/bootstrap.min.css" integrity="sha384-B0vP5xmATw1+K9KRQjQERJvTumQW0nPEzvF6L/Z6nronJ3oUOFUFpCjEUQouq2+l" crossorigin="anonymous"&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;link</t>
+  </si>
+  <si>
+    <t>    rel="stylesheet"</t>
+  </si>
+  <si>
+    <t>    href="https://pro.fontawesome.com/releases/v5.10.0/css/all.css"</t>
+  </si>
+  <si>
+    <t>    integrity="sha384-AYmEC3Yw5cVb3ZcuHtOA93w35dYTsvhLPVnYs9eStHfGJvOvKxVfELGroGkvsg+p"</t>
+  </si>
+  <si>
+    <t>    crossorigin="anonymous"/&gt;</t>
+  </si>
+  <si>
+    <t>add CSS</t>
+  </si>
+  <si>
+    <t>add Boottrap, FontAwesome, Jquery</t>
+  </si>
+  <si>
+    <t>ADD file JS</t>
+  </si>
+  <si>
+    <t>Đầu tiên xem file index.js trong folder : router để thấy nó sẽ kích hoạt component nào</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,8 +148,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,6 +195,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -106,16 +220,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -282,6 +408,287 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>102990</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>160976</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F272276A-4B0E-4AC5-AF70-FDB5C6D9204D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="20716875"/>
+          <a:ext cx="14276190" cy="7590476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>184</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA668EBB-BCFC-458C-A638-8E96646CD08D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5419725" y="25298400"/>
+          <a:ext cx="2686050" cy="3333750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>217</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>379244</xdr:colOff>
+      <xdr:row>263</xdr:row>
+      <xdr:rowOff>17974</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA9DB110-9148-4F03-A545-742B141A3CDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1724025" y="31746825"/>
+          <a:ext cx="14047619" cy="8609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>268</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>408346</xdr:colOff>
+      <xdr:row>313</xdr:row>
+      <xdr:rowOff>37027</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="15" name="Group 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08335EC7-844C-42E8-AB52-14B9CA655BA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1838325" y="51796950"/>
+          <a:ext cx="19448821" cy="8580952"/>
+          <a:chOff x="1828800" y="51577875"/>
+          <a:chExt cx="19448821" cy="8580952"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="12" name="Picture 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B0BAA8E-9C1B-48FB-B9C0-ADF26D37EDC4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1828800" y="51577875"/>
+            <a:ext cx="17142857" cy="8580952"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="13" name="Picture 12">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56277294-1213-4003-8895-40280FBCEC7A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11449050" y="53320950"/>
+            <a:ext cx="9828571" cy="4523809"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>226647</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>151309</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{952E421D-6975-4AA1-A196-A6F8106E3256}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="20716875"/>
+          <a:ext cx="15619047" cy="8723809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -550,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D12:L36"/>
+  <dimension ref="D12:AB266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="J86" sqref="J86"/>
+    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
+      <selection activeCell="D318" sqref="D318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +1029,7 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -633,7 +1040,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
         <v>5</v>
@@ -646,7 +1053,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -659,7 +1066,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -670,7 +1077,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -683,7 +1090,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -694,24 +1101,27 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
-    </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D26" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E26" s="2">
         <v>1</v>
@@ -726,13 +1136,13 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="E27" s="2">
         <v>2</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -741,11 +1151,11 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -754,7 +1164,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -765,7 +1175,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -776,7 +1186,7 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -787,7 +1197,7 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -842,9 +1252,426 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="4:5" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D87" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E91" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="92" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E92" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E94" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D98" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E98" s="4"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="4"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="4"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="4"/>
+      <c r="L98" s="4"/>
+    </row>
+    <row r="101" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D101" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="105" spans="4:21" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D105" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E105" s="10"/>
+      <c r="F105" s="10"/>
+      <c r="G105" s="10"/>
+      <c r="H105" s="10"/>
+      <c r="I105" s="10"/>
+      <c r="J105" s="11"/>
+      <c r="K105" s="11"/>
+      <c r="L105" s="11"/>
+      <c r="M105" s="11"/>
+      <c r="N105" s="11"/>
+      <c r="O105" s="11"/>
+      <c r="P105" s="11"/>
+      <c r="Q105" s="11"/>
+      <c r="R105" s="11"/>
+      <c r="S105" s="11"/>
+      <c r="T105" s="11"/>
+      <c r="U105" s="11"/>
+    </row>
+    <row r="159" spans="4:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D159" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E159" s="10"/>
+      <c r="F159" s="10"/>
+      <c r="G159" s="10"/>
+      <c r="H159" s="10"/>
+      <c r="I159" s="10"/>
+    </row>
+    <row r="202" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="F202" s="1"/>
+      <c r="G202" s="1"/>
+      <c r="H202" s="1"/>
+      <c r="I202" s="1"/>
+      <c r="J202" s="1"/>
+      <c r="K202" s="1"/>
+      <c r="L202" s="1"/>
+      <c r="M202" s="1"/>
+      <c r="N202" s="1"/>
+      <c r="O202" s="1"/>
+      <c r="P202" s="1"/>
+      <c r="Q202" s="1"/>
+      <c r="R202" s="1"/>
+      <c r="S202" s="1"/>
+      <c r="T202" s="1"/>
+      <c r="U202" s="1"/>
+      <c r="V202" s="1"/>
+      <c r="W202" s="1"/>
+      <c r="X202" s="1"/>
+      <c r="Y202" s="1"/>
+      <c r="Z202" s="1"/>
+      <c r="AA202" s="1"/>
+      <c r="AB202" s="1"/>
+    </row>
+    <row r="203" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="F203" s="1"/>
+      <c r="G203" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H203" s="9"/>
+      <c r="I203" s="9"/>
+      <c r="J203" s="9"/>
+      <c r="K203" s="9"/>
+      <c r="L203" s="9"/>
+      <c r="M203" s="9"/>
+      <c r="N203" s="9"/>
+      <c r="O203" s="9"/>
+      <c r="P203" s="9"/>
+      <c r="Q203" s="9"/>
+      <c r="R203" s="9"/>
+      <c r="S203" s="9"/>
+      <c r="T203" s="9"/>
+      <c r="U203" s="9"/>
+      <c r="V203" s="9"/>
+      <c r="W203" s="9"/>
+      <c r="X203" s="9"/>
+      <c r="Y203" s="1"/>
+      <c r="Z203" s="1"/>
+      <c r="AA203" s="1"/>
+      <c r="AB203" s="1"/>
+    </row>
+    <row r="204" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="F204" s="1"/>
+      <c r="G204" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H204" s="9"/>
+      <c r="I204" s="9"/>
+      <c r="J204" s="9"/>
+      <c r="K204" s="9"/>
+      <c r="L204" s="9"/>
+      <c r="M204" s="9"/>
+      <c r="N204" s="9"/>
+      <c r="O204" s="9"/>
+      <c r="P204" s="9"/>
+      <c r="Q204" s="9"/>
+      <c r="R204" s="9"/>
+      <c r="S204" s="9"/>
+      <c r="T204" s="9"/>
+      <c r="U204" s="9"/>
+      <c r="V204" s="9"/>
+      <c r="W204" s="9"/>
+      <c r="X204" s="9"/>
+      <c r="Y204" s="1"/>
+      <c r="Z204" s="1"/>
+      <c r="AA204" s="1"/>
+      <c r="AB204" s="1"/>
+    </row>
+    <row r="205" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="F205" s="1"/>
+      <c r="G205" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H205" s="9"/>
+      <c r="I205" s="9"/>
+      <c r="J205" s="9"/>
+      <c r="K205" s="9"/>
+      <c r="L205" s="9"/>
+      <c r="M205" s="9"/>
+      <c r="N205" s="9"/>
+      <c r="O205" s="9"/>
+      <c r="P205" s="9"/>
+      <c r="Q205" s="9"/>
+      <c r="R205" s="9"/>
+      <c r="S205" s="9"/>
+      <c r="T205" s="9"/>
+      <c r="U205" s="9"/>
+      <c r="V205" s="9"/>
+      <c r="W205" s="9"/>
+      <c r="X205" s="9"/>
+      <c r="Y205" s="1"/>
+      <c r="Z205" s="1"/>
+      <c r="AA205" s="1"/>
+      <c r="AB205" s="1"/>
+    </row>
+    <row r="206" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="F206" s="1"/>
+      <c r="G206" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H206" s="9"/>
+      <c r="I206" s="9"/>
+      <c r="J206" s="9"/>
+      <c r="K206" s="9"/>
+      <c r="L206" s="9"/>
+      <c r="M206" s="9"/>
+      <c r="N206" s="9"/>
+      <c r="O206" s="9"/>
+      <c r="P206" s="9"/>
+      <c r="Q206" s="9"/>
+      <c r="R206" s="9"/>
+      <c r="S206" s="9"/>
+      <c r="T206" s="9"/>
+      <c r="U206" s="9"/>
+      <c r="V206" s="9"/>
+      <c r="W206" s="9"/>
+      <c r="X206" s="9"/>
+      <c r="Y206" s="1"/>
+      <c r="Z206" s="1"/>
+      <c r="AA206" s="1"/>
+      <c r="AB206" s="1"/>
+    </row>
+    <row r="207" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="F207" s="1"/>
+      <c r="G207" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H207" s="9"/>
+      <c r="I207" s="9"/>
+      <c r="J207" s="9"/>
+      <c r="K207" s="9"/>
+      <c r="L207" s="9"/>
+      <c r="M207" s="9"/>
+      <c r="N207" s="9"/>
+      <c r="O207" s="9"/>
+      <c r="P207" s="9"/>
+      <c r="Q207" s="9"/>
+      <c r="R207" s="9"/>
+      <c r="S207" s="9"/>
+      <c r="T207" s="9"/>
+      <c r="U207" s="9"/>
+      <c r="V207" s="9"/>
+      <c r="W207" s="9"/>
+      <c r="X207" s="9"/>
+      <c r="Y207" s="1"/>
+      <c r="Z207" s="1"/>
+      <c r="AA207" s="1"/>
+      <c r="AB207" s="1"/>
+    </row>
+    <row r="208" spans="6:28" x14ac:dyDescent="0.25">
+      <c r="F208" s="1"/>
+      <c r="G208" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H208" s="9"/>
+      <c r="I208" s="9"/>
+      <c r="J208" s="9"/>
+      <c r="K208" s="9"/>
+      <c r="L208" s="9"/>
+      <c r="M208" s="9"/>
+      <c r="N208" s="9"/>
+      <c r="O208" s="9"/>
+      <c r="P208" s="9"/>
+      <c r="Q208" s="9"/>
+      <c r="R208" s="9"/>
+      <c r="S208" s="9"/>
+      <c r="T208" s="9"/>
+      <c r="U208" s="9"/>
+      <c r="V208" s="9"/>
+      <c r="W208" s="9"/>
+      <c r="X208" s="9"/>
+      <c r="Y208" s="1"/>
+      <c r="Z208" s="1"/>
+      <c r="AA208" s="1"/>
+      <c r="AB208" s="1"/>
+    </row>
+    <row r="209" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="F209" s="1"/>
+      <c r="G209" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H209" s="9"/>
+      <c r="I209" s="9"/>
+      <c r="J209" s="9"/>
+      <c r="K209" s="9"/>
+      <c r="L209" s="9"/>
+      <c r="M209" s="9"/>
+      <c r="N209" s="9"/>
+      <c r="O209" s="9"/>
+      <c r="P209" s="9"/>
+      <c r="Q209" s="9"/>
+      <c r="R209" s="9"/>
+      <c r="S209" s="9"/>
+      <c r="T209" s="9"/>
+      <c r="U209" s="9"/>
+      <c r="V209" s="9"/>
+      <c r="W209" s="9"/>
+      <c r="X209" s="9"/>
+      <c r="Y209" s="1"/>
+      <c r="Z209" s="1"/>
+      <c r="AA209" s="1"/>
+      <c r="AB209" s="1"/>
+    </row>
+    <row r="210" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="F210" s="1"/>
+      <c r="G210" s="9"/>
+      <c r="H210" s="9"/>
+      <c r="I210" s="9"/>
+      <c r="J210" s="9"/>
+      <c r="K210" s="9"/>
+      <c r="L210" s="9"/>
+      <c r="M210" s="9"/>
+      <c r="N210" s="9"/>
+      <c r="O210" s="9"/>
+      <c r="P210" s="9"/>
+      <c r="Q210" s="9"/>
+      <c r="R210" s="9"/>
+      <c r="S210" s="9"/>
+      <c r="T210" s="9"/>
+      <c r="U210" s="9"/>
+      <c r="V210" s="9"/>
+      <c r="W210" s="9"/>
+      <c r="X210" s="9"/>
+      <c r="Y210" s="1"/>
+      <c r="Z210" s="1"/>
+      <c r="AA210" s="1"/>
+      <c r="AB210" s="1"/>
+    </row>
+    <row r="211" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="F211" s="1"/>
+      <c r="G211" s="1"/>
+      <c r="H211" s="1"/>
+      <c r="I211" s="1"/>
+      <c r="J211" s="1"/>
+      <c r="K211" s="1"/>
+      <c r="L211" s="1"/>
+      <c r="M211" s="1"/>
+      <c r="N211" s="1"/>
+      <c r="O211" s="1"/>
+      <c r="P211" s="1"/>
+      <c r="Q211" s="1"/>
+      <c r="R211" s="1"/>
+      <c r="S211" s="1"/>
+      <c r="T211" s="1"/>
+      <c r="U211" s="1"/>
+      <c r="V211" s="1"/>
+      <c r="W211" s="1"/>
+      <c r="X211" s="1"/>
+      <c r="Y211" s="1"/>
+      <c r="Z211" s="1"/>
+      <c r="AA211" s="1"/>
+      <c r="AB211" s="1"/>
+    </row>
+    <row r="212" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="F212" s="1"/>
+      <c r="G212" s="1"/>
+      <c r="H212" s="1"/>
+      <c r="I212" s="1"/>
+      <c r="J212" s="1"/>
+      <c r="K212" s="1"/>
+      <c r="L212" s="1"/>
+      <c r="M212" s="1"/>
+      <c r="N212" s="1"/>
+      <c r="O212" s="1"/>
+      <c r="P212" s="1"/>
+      <c r="Q212" s="1"/>
+      <c r="R212" s="1"/>
+      <c r="S212" s="1"/>
+      <c r="T212" s="1"/>
+      <c r="U212" s="1"/>
+      <c r="V212" s="1"/>
+      <c r="W212" s="1"/>
+      <c r="X212" s="1"/>
+      <c r="Y212" s="1"/>
+      <c r="Z212" s="1"/>
+      <c r="AA212" s="1"/>
+      <c r="AB212" s="1"/>
+    </row>
+    <row r="213" spans="4:28" x14ac:dyDescent="0.25">
+      <c r="F213" s="1"/>
+      <c r="G213" s="1"/>
+      <c r="H213" s="1"/>
+      <c r="I213" s="1"/>
+      <c r="J213" s="1"/>
+      <c r="K213" s="1"/>
+      <c r="L213" s="1"/>
+      <c r="M213" s="1"/>
+      <c r="N213" s="1"/>
+      <c r="O213" s="1"/>
+      <c r="P213" s="1"/>
+      <c r="Q213" s="1"/>
+      <c r="R213" s="1"/>
+      <c r="S213" s="1"/>
+      <c r="T213" s="1"/>
+      <c r="U213" s="1"/>
+      <c r="V213" s="1"/>
+      <c r="W213" s="1"/>
+      <c r="X213" s="1"/>
+      <c r="Y213" s="1"/>
+      <c r="Z213" s="1"/>
+      <c r="AA213" s="1"/>
+      <c r="AB213" s="1"/>
+    </row>
+    <row r="217" spans="4:28" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D217" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="266" spans="4:4" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D266" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D101" r:id="rId1" xr:uid="{7BDF3BBB-DE4A-4EA2-8FA2-4E8EDB0FEBE0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
create project v.2 finish data.json, xem file NOTE.xlsx phần GEN DATA
create project v.2 finish data.json, xem file NOTE.xlsx phần GEN DATA
</commit_message>
<xml_diff>
--- a/NOTE.xlsx
+++ b/NOTE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\LEARNING\VUEJS\Vue3EShopSolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B2FEAB-79B3-4190-976E-79F5511A885D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9499B5EE-768E-47DF-A1FC-4EB304A1C6CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Set-ExecutionPolicy -Scope Process -ExecutionPolicy Bypass</t>
   </si>
@@ -127,13 +127,25 @@
   </si>
   <si>
     <t>Đầu tiên xem file index.js trong folder : router để thấy nó sẽ kích hoạt component nào</t>
+  </si>
+  <si>
+    <t>https://www.codota.com/setup/vscode</t>
+  </si>
+  <si>
+    <t>GEN DATA</t>
+  </si>
+  <si>
+    <t>node genData.js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mở riêng 1 project nodeJS lên rồi chạy file </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +196,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -224,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -239,6 +258,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -285,7 +307,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3857625" y="3305175"/>
+          <a:off x="3857625" y="3590925"/>
           <a:ext cx="15982106" cy="11057414"/>
           <a:chOff x="3200400" y="3971925"/>
           <a:chExt cx="15982106" cy="11057414"/>
@@ -580,7 +602,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1838325" y="51796950"/>
+          <a:off x="1838325" y="52082700"/>
           <a:ext cx="19448821" cy="8580952"/>
           <a:chOff x="1828800" y="51577875"/>
           <a:chExt cx="19448821" cy="8580952"/>
@@ -689,6 +711,150 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>323</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>408362</xdr:colOff>
+      <xdr:row>333</xdr:row>
+      <xdr:rowOff>171190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3840D3FB-588D-45B7-8580-112E3CD7D15F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="62674500"/>
+          <a:ext cx="9704762" cy="2076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>334</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>46386</xdr:colOff>
+      <xdr:row>344</xdr:row>
+      <xdr:rowOff>66413</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C606EE2-BE3D-4FDC-8628-D9C30F5D5B5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866900" y="64931925"/>
+          <a:ext cx="9914286" cy="2095238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>330</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>342</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0464C307-518A-4DD6-999A-F7B1402139B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3228975" y="64217550"/>
+          <a:ext cx="5172075" cy="2371725"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -957,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D12:AB266"/>
+  <dimension ref="D5:AB337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="B221" sqref="B221"/>
+    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
+      <selection activeCell="D319" sqref="D319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,6 +1134,28 @@
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="5" spans="4:12" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+    </row>
+    <row r="6" spans="4:12" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+    </row>
     <row r="12" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
         <v>8</v>
@@ -1666,6 +1854,29 @@
         <v>32</v>
       </c>
     </row>
+    <row r="319" spans="4:4" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D319" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="321" spans="4:14" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D321" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E321" s="13"/>
+      <c r="F321" s="13"/>
+      <c r="G321" s="13"/>
+      <c r="H321" s="13"/>
+      <c r="K321" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="L321" s="14"/>
+      <c r="M321" s="14"/>
+      <c r="N321" s="5"/>
+    </row>
+    <row r="337" spans="4:4" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D337" s="13"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D101" r:id="rId1" xr:uid="{7BDF3BBB-DE4A-4EA2-8FA2-4E8EDB0FEBE0}"/>

</xml_diff>

<commit_message>
learning Vuex3  1.0 STATE
learning Vuex3  1.0 STATE
</commit_message>
<xml_diff>
--- a/NOTE.xlsx
+++ b/NOTE.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\LEARNING\VUEJS\Vue3EShopSolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9499B5EE-768E-47DF-A1FC-4EB304A1C6CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D1A242-DDB0-41D1-8874-57FF91B3FAE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3255" yWindow="2565" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="VUEX 3" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Set-ExecutionPolicy -Scope Process -ExecutionPolicy Bypass</t>
   </si>
@@ -139,6 +140,15 @@
   </si>
   <si>
     <t xml:space="preserve">mở riêng 1 project nodeJS lên rồi chạy file </t>
+  </si>
+  <si>
+    <t>https://learnvue.co/2020/12/how-to-use-lifecycle-hooks-in-vue3/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=y7DQhNs9Azw&amp;t=10s&amp;ab_channel=LaithHarbLaithHarb</t>
+  </si>
+  <si>
+    <t>https://next.vuex.vuejs.org/guide/migrating-to-4-0-from-3-x.html#installation-process</t>
   </si>
 </sst>
 </file>
@@ -1123,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D5:AB337"/>
+  <dimension ref="D2:AB337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
-      <selection activeCell="D319" sqref="D319"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,6 +1144,11 @@
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D2" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="5" spans="4:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="D5" s="12" t="s">
         <v>34</v>
@@ -1880,9 +1895,38 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D101" r:id="rId1" xr:uid="{7BDF3BBB-DE4A-4EA2-8FA2-4E8EDB0FEBE0}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{C639B9B3-7B8B-43BD-8A28-E6EBC28E2721}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B9DC6D4-3C33-4D3C-9BA7-CB27A94A316A}">
+  <dimension ref="C7:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1" xr:uid="{328023CB-B288-48BD-A32B-CD672AAE26AA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
learning Vuex4  2.0 STATE
learning Vuex4  2.0 STATE
</commit_message>
<xml_diff>
--- a/NOTE.xlsx
+++ b/NOTE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\LEARNING\VUEJS\Vue3EShopSolution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\Vue\Vue3EShopSolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D1A242-DDB0-41D1-8874-57FF91B3FAE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9EDCD0-B800-4C57-888E-AE00F50D7518}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3255" yWindow="2565" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Set-ExecutionPolicy -Scope Process -ExecutionPolicy Bypass</t>
   </si>
@@ -149,6 +149,18 @@
   </si>
   <si>
     <t>https://next.vuex.vuejs.org/guide/migrating-to-4-0-from-3-x.html#installation-process</t>
+  </si>
+  <si>
+    <t>Getter chay 2 way binding</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>mutation chay  để thay đổi trực tiếp state</t>
+  </si>
+  <si>
+    <t>actión :  có thể thực hiện gọi service hay axios update lên state</t>
   </si>
 </sst>
 </file>
@@ -870,6 +882,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>46705</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>104190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A2C31FF-CB63-493F-80B0-627DB5867A13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="3429000"/>
+          <a:ext cx="7361905" cy="4676190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1135,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D2:AB337"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A322" workbookViewId="0">
+      <selection activeCell="M319" sqref="M319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,28 +1966,78 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B9DC6D4-3C33-4D3C-9BA7-CB27A94A316A}">
-  <dimension ref="C7:C10"/>
+  <dimension ref="C7:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="7" t="s">
         <v>39</v>
       </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" xr:uid="{328023CB-B288-48BD-A32B-CD672AAE26AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
example insert, delete, update fireBase
example insert, delete, update fireBase
</commit_message>
<xml_diff>
--- a/NOTE.xlsx
+++ b/NOTE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\Vue\Vue3EShopSolution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\LEARNING\VUEJS\Vue3EShopSolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6340C92E-991A-4263-8E6E-5D31C476E3DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4AACDD-203A-4712-BF2D-A4914ECFF48D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
   <si>
     <t>Set-ExecutionPolicy -Scope Process -ExecutionPolicy Bypass</t>
   </si>
@@ -179,13 +179,172 @@
   </si>
   <si>
     <t>HTML CSS</t>
+  </si>
+  <si>
+    <t>// https://console.firebase.google.com/</t>
+  </si>
+  <si>
+    <t>// For Firebase JS SDK v7.20.0 and later, measurementId is optional</t>
+  </si>
+  <si>
+    <t>// lqvinh.hsu@gmail.com</t>
+  </si>
+  <si>
+    <t>// console.firebase   = app named : "vueLearning-live-chat"</t>
+  </si>
+  <si>
+    <t>quan tâm đến rule có khi sẽ bị lỗi, do trong rule yêu cầu authencicate mà bên ngoài ko biết, cứ thao tác data với FB là bị lỗi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  }</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>rules_version = '2';</t>
+  </si>
+  <si>
+    <t>service cloud.firestore {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  match /databases/{database}/documents {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    match /playlists/{docId} {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      allow read, create: if request.auth != null;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      allow delete, update: if request.auth.uid == resource.data.userId;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    match /{document=**} {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      allow read, write: if true;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    const HandleRegister = async () =&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         const dataNew = {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          name :'name1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          testJobs: [],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          createdAt: timestamp(),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        };</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       const res = await AddDocHandle(dataNew);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (!error.value) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            const res2 = res.id;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        }</t>
+  </si>
+  <si>
+    <t>Yêu cầu authenticate</t>
+  </si>
+  <si>
+    <t>không cần authenticate</t>
+  </si>
+  <si>
+    <t>INSERT DOC</t>
+  </si>
+  <si>
+    <t>DELETE DOC</t>
+  </si>
+  <si>
+    <t>const { AddDocHandle, error, isPending } = AddDoc("DOCTest");</t>
+  </si>
+  <si>
+    <t>import AddDoc from "../src/services/fireBase/AddDoc.js";</t>
+  </si>
+  <si>
+    <t>import { timestamp } from "../src/services/fireBase/config";</t>
+  </si>
+  <si>
+    <t>          }</t>
+  </si>
+  <si>
+    <t>      };</t>
+  </si>
+  <si>
+    <t>      const { DeleteDocHandle, error, isPending} = DeleteDoc("DOCTest", 'LGAvxF26bg4FXdGbIwvK');</t>
+  </si>
+  <si>
+    <t>      const HandleRegister = async () =&gt;{</t>
+  </si>
+  <si>
+    <t>          const resDelete = await DeleteDocHandle();</t>
+  </si>
+  <si>
+    <t>          if (!error.value) {</t>
+  </si>
+  <si>
+    <t>            const res2 = resDelete;</t>
+  </si>
+  <si>
+    <t>import DeleteDoc from "../src/services/fireBase/DeleteDoc";</t>
+  </si>
+  <si>
+    <t>UPDATE DOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> const { UpdateDocHandle, error, isPending } = UpdateDoc("DOCTest", 'WM8DNCaXPylf1dUwtLhb');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          const dataUpdate = {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            name : 'nameUpdate',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            testJobs : ['1','2'],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          const resUpd = await UpdateDocHandle(dataUpdate);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      };</t>
+  </si>
+  <si>
+    <t>const HandleRegister = async () =&gt;{</t>
+  </si>
+  <si>
+    <t>import UpdateDoc from "../src/services/fireBase/UpdateDoc";</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +402,88 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF374747"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF374747"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -283,7 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -301,6 +542,41 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -317,6 +593,14 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D124-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
+</file>
+
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D124-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -897,6 +1181,247 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>378</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>93696</xdr:colOff>
+      <xdr:row>407</xdr:row>
+      <xdr:rowOff>123126</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A0130F1-FF96-4598-A6D6-7BF3681C619F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1838325" y="73609200"/>
+          <a:ext cx="12428571" cy="5590476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>373</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>393</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C4F2022-BC1C-4901-A367-1C2CAF159E9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10620375" y="72523350"/>
+          <a:ext cx="762000" cy="3771900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>24</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>392</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>28</xdr:col>
+          <xdr:colOff>447675</xdr:colOff>
+          <xdr:row>396</xdr:row>
+          <xdr:rowOff>123825</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Control 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CE957D0-FDCD-4DFC-B432-3FFC1F06A9FF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>24</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>393</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>28</xdr:col>
+          <xdr:colOff>447675</xdr:colOff>
+          <xdr:row>397</xdr:row>
+          <xdr:rowOff>123825</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Control 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{356671FE-37AD-4A49-B572-F69BF9DE7849}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>414</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>485359</xdr:colOff>
+      <xdr:row>440</xdr:row>
+      <xdr:rowOff>8912</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{014F7BE6-C275-4FDF-8CB2-573C50A264EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2800350" y="80352900"/>
+          <a:ext cx="3323809" cy="4904762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1211,24 +1736,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D2:AB363"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="D2:AF472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A343" workbookViewId="0">
-      <selection activeCell="L361" sqref="L361"/>
+    <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
+      <selection activeCell="D474" sqref="D474"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:12">
       <c r="D2" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="4:12" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="4:12" ht="26.25">
       <c r="D5" s="12" t="s">
         <v>34</v>
       </c>
@@ -1240,7 +1766,7 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="4:12" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="4:12" ht="26.25">
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
@@ -1250,7 +1776,7 @@
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
     </row>
-    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:12">
       <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1263,7 +1789,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:12">
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
         <v>1</v>
@@ -1276,7 +1802,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:12">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1287,7 +1813,7 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:12">
       <c r="D15" s="1"/>
       <c r="E15" s="2" t="s">
         <v>2</v>
@@ -1300,7 +1826,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:12">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1311,7 +1837,7 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:14">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1322,7 +1848,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:14">
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
         <v>5</v>
@@ -1335,7 +1861,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:14">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1348,7 +1874,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:14">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1359,7 +1885,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:14">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1372,7 +1898,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:14">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1383,7 +1909,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:14">
       <c r="D25" s="1" t="s">
         <v>4</v>
       </c>
@@ -1401,7 +1927,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:14">
       <c r="D26" s="3" t="s">
         <v>9</v>
       </c>
@@ -1418,7 +1944,7 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:14">
       <c r="D27" s="1"/>
       <c r="E27" s="2">
         <v>2</v>
@@ -1433,7 +1959,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:14">
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
@@ -1446,7 +1972,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:14">
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1457,7 +1983,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:14">
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1468,7 +1994,7 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:14">
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1479,7 +2005,7 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:14">
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1490,7 +2016,7 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:12">
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -1501,7 +2027,7 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:12">
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -1512,7 +2038,7 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:12">
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -1523,7 +2049,7 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:12">
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -1534,47 +2060,47 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:4">
       <c r="D80" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:5">
       <c r="E81" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="4:5" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="87" spans="4:5" ht="26.25">
       <c r="D87" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:5">
       <c r="D88" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:5">
       <c r="E91" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:5">
       <c r="E92" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:5">
       <c r="E93" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:5">
       <c r="E94" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:21">
       <c r="D98" s="4" t="s">
         <v>21</v>
       </c>
@@ -1587,12 +2113,12 @@
       <c r="K98" s="4"/>
       <c r="L98" s="4"/>
     </row>
-    <row r="101" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:21">
       <c r="D101" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="105" spans="4:21" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="105" spans="4:21" ht="26.25">
       <c r="D105" s="10" t="s">
         <v>33</v>
       </c>
@@ -1614,7 +2140,7 @@
       <c r="T105" s="11"/>
       <c r="U105" s="11"/>
     </row>
-    <row r="159" spans="4:9" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="159" spans="4:9" ht="26.25">
       <c r="D159" s="10" t="s">
         <v>31</v>
       </c>
@@ -1624,7 +2150,7 @@
       <c r="H159" s="10"/>
       <c r="I159" s="10"/>
     </row>
-    <row r="202" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="202" spans="6:28">
       <c r="F202" s="1"/>
       <c r="G202" s="1"/>
       <c r="H202" s="1"/>
@@ -1649,7 +2175,7 @@
       <c r="AA202" s="1"/>
       <c r="AB202" s="1"/>
     </row>
-    <row r="203" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="203" spans="6:28">
       <c r="F203" s="1"/>
       <c r="G203" s="8" t="s">
         <v>23</v>
@@ -1676,7 +2202,7 @@
       <c r="AA203" s="1"/>
       <c r="AB203" s="1"/>
     </row>
-    <row r="204" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="204" spans="6:28">
       <c r="F204" s="1"/>
       <c r="G204" s="8" t="s">
         <v>24</v>
@@ -1703,7 +2229,7 @@
       <c r="AA204" s="1"/>
       <c r="AB204" s="1"/>
     </row>
-    <row r="205" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="205" spans="6:28">
       <c r="F205" s="1"/>
       <c r="G205" s="8" t="s">
         <v>25</v>
@@ -1730,7 +2256,7 @@
       <c r="AA205" s="1"/>
       <c r="AB205" s="1"/>
     </row>
-    <row r="206" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="206" spans="6:28">
       <c r="F206" s="1"/>
       <c r="G206" s="8" t="s">
         <v>26</v>
@@ -1757,7 +2283,7 @@
       <c r="AA206" s="1"/>
       <c r="AB206" s="1"/>
     </row>
-    <row r="207" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="207" spans="6:28">
       <c r="F207" s="1"/>
       <c r="G207" s="8" t="s">
         <v>27</v>
@@ -1784,7 +2310,7 @@
       <c r="AA207" s="1"/>
       <c r="AB207" s="1"/>
     </row>
-    <row r="208" spans="6:28" x14ac:dyDescent="0.25">
+    <row r="208" spans="6:28">
       <c r="F208" s="1"/>
       <c r="G208" s="8" t="s">
         <v>28</v>
@@ -1811,7 +2337,7 @@
       <c r="AA208" s="1"/>
       <c r="AB208" s="1"/>
     </row>
-    <row r="209" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="209" spans="4:28">
       <c r="F209" s="1"/>
       <c r="G209" s="8" t="s">
         <v>29</v>
@@ -1838,7 +2364,7 @@
       <c r="AA209" s="1"/>
       <c r="AB209" s="1"/>
     </row>
-    <row r="210" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="210" spans="4:28">
       <c r="F210" s="1"/>
       <c r="G210" s="9"/>
       <c r="H210" s="9"/>
@@ -1863,7 +2389,7 @@
       <c r="AA210" s="1"/>
       <c r="AB210" s="1"/>
     </row>
-    <row r="211" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="211" spans="4:28">
       <c r="F211" s="1"/>
       <c r="G211" s="1"/>
       <c r="H211" s="1"/>
@@ -1888,7 +2414,7 @@
       <c r="AA211" s="1"/>
       <c r="AB211" s="1"/>
     </row>
-    <row r="212" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="212" spans="4:28">
       <c r="F212" s="1"/>
       <c r="G212" s="1"/>
       <c r="H212" s="1"/>
@@ -1913,7 +2439,7 @@
       <c r="AA212" s="1"/>
       <c r="AB212" s="1"/>
     </row>
-    <row r="213" spans="4:28" x14ac:dyDescent="0.25">
+    <row r="213" spans="4:28">
       <c r="F213" s="1"/>
       <c r="G213" s="1"/>
       <c r="H213" s="1"/>
@@ -1938,22 +2464,22 @@
       <c r="AA213" s="1"/>
       <c r="AB213" s="1"/>
     </row>
-    <row r="217" spans="4:28" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="217" spans="4:28" ht="26.25">
       <c r="D217" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="266" spans="4:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="266" spans="4:4" ht="26.25">
       <c r="D266" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="319" spans="4:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="319" spans="4:4" ht="26.25">
       <c r="D319" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="321" spans="4:14" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="321" spans="4:14" ht="26.25">
       <c r="D321" s="13" t="s">
         <v>37</v>
       </c>
@@ -1968,20 +2494,20 @@
       <c r="M321" s="14"/>
       <c r="N321" s="5"/>
     </row>
-    <row r="337" spans="4:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="337" spans="4:4" ht="26.25">
       <c r="D337" s="13"/>
     </row>
-    <row r="352" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="352" spans="4:4">
       <c r="D352" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="357" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="357" spans="4:12">
       <c r="D357" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="360" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="360" spans="4:12">
       <c r="D360" t="s">
         <v>47</v>
       </c>
@@ -1989,15 +2515,1055 @@
         <v>50</v>
       </c>
     </row>
-    <row r="361" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="361" spans="4:12">
       <c r="D361" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="363" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="363" spans="4:12">
       <c r="D363" t="s">
         <v>49</v>
       </c>
+    </row>
+    <row r="372" spans="4:30">
+      <c r="D372" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E372" s="9"/>
+      <c r="F372" s="9"/>
+      <c r="G372" s="9"/>
+      <c r="H372" s="9"/>
+      <c r="I372" s="9"/>
+      <c r="J372" s="9"/>
+      <c r="K372" s="9"/>
+      <c r="L372" s="9"/>
+      <c r="M372" s="9"/>
+      <c r="N372" s="9"/>
+    </row>
+    <row r="373" spans="4:30">
+      <c r="D373" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E373" s="9"/>
+      <c r="F373" s="9"/>
+      <c r="G373" s="9"/>
+      <c r="H373" s="9"/>
+      <c r="I373" s="9"/>
+      <c r="J373" s="9"/>
+      <c r="K373" s="9"/>
+      <c r="L373" s="9"/>
+      <c r="M373" s="9"/>
+      <c r="N373" s="9"/>
+      <c r="P373" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q373" s="16"/>
+      <c r="R373" s="16"/>
+      <c r="S373" s="16"/>
+      <c r="T373" s="16"/>
+      <c r="U373" s="16"/>
+      <c r="V373" s="16"/>
+      <c r="W373" s="16"/>
+      <c r="X373" s="16"/>
+      <c r="Y373" s="16"/>
+      <c r="Z373" s="16"/>
+      <c r="AA373" s="16"/>
+      <c r="AB373" s="16"/>
+    </row>
+    <row r="374" spans="4:30">
+      <c r="D374" s="15"/>
+      <c r="E374" s="9"/>
+      <c r="F374" s="9"/>
+      <c r="G374" s="9"/>
+      <c r="H374" s="9"/>
+      <c r="I374" s="9"/>
+      <c r="J374" s="9"/>
+      <c r="K374" s="9"/>
+      <c r="L374" s="9"/>
+      <c r="M374" s="9"/>
+      <c r="N374" s="9"/>
+      <c r="P374" s="16"/>
+      <c r="Q374" s="16"/>
+      <c r="R374" s="16"/>
+      <c r="S374" s="16"/>
+      <c r="T374" s="16"/>
+      <c r="U374" s="16"/>
+      <c r="V374" s="16"/>
+      <c r="W374" s="16"/>
+      <c r="X374" s="16"/>
+      <c r="Y374" s="16"/>
+      <c r="Z374" s="16"/>
+      <c r="AA374" s="16"/>
+      <c r="AB374" s="16"/>
+    </row>
+    <row r="375" spans="4:30">
+      <c r="D375" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E375" s="9"/>
+      <c r="F375" s="9"/>
+      <c r="G375" s="9"/>
+      <c r="H375" s="9"/>
+      <c r="I375" s="9"/>
+      <c r="J375" s="9"/>
+      <c r="K375" s="9"/>
+      <c r="L375" s="9"/>
+      <c r="M375" s="9"/>
+      <c r="N375" s="9"/>
+    </row>
+    <row r="376" spans="4:30" ht="19.5">
+      <c r="D376" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E376" s="9"/>
+      <c r="F376" s="9"/>
+      <c r="G376" s="9"/>
+      <c r="H376" s="9"/>
+      <c r="I376" s="9"/>
+      <c r="J376" s="9"/>
+      <c r="K376" s="9"/>
+      <c r="L376" s="9"/>
+      <c r="M376" s="9"/>
+      <c r="N376" s="9"/>
+      <c r="X376" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y376" s="22"/>
+      <c r="Z376" s="22"/>
+    </row>
+    <row r="377" spans="4:30">
+      <c r="D377" s="9"/>
+      <c r="E377" s="9"/>
+      <c r="F377" s="9"/>
+      <c r="G377" s="9"/>
+      <c r="H377" s="9"/>
+      <c r="I377" s="9"/>
+      <c r="J377" s="9"/>
+      <c r="K377" s="9"/>
+      <c r="L377" s="9"/>
+      <c r="M377" s="9"/>
+      <c r="N377" s="9"/>
+      <c r="X377" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y377" s="4"/>
+      <c r="Z377" s="4"/>
+      <c r="AA377" s="4"/>
+      <c r="AB377" s="4"/>
+      <c r="AC377" s="4"/>
+      <c r="AD377" s="4"/>
+    </row>
+    <row r="378" spans="4:30">
+      <c r="X378" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y378" s="4"/>
+      <c r="Z378" s="4"/>
+      <c r="AA378" s="4"/>
+      <c r="AB378" s="4"/>
+      <c r="AC378" s="4"/>
+      <c r="AD378" s="4"/>
+    </row>
+    <row r="379" spans="4:30">
+      <c r="X379" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y379" s="4"/>
+      <c r="Z379" s="4"/>
+      <c r="AA379" s="4"/>
+      <c r="AB379" s="4"/>
+      <c r="AC379" s="4"/>
+      <c r="AD379" s="4"/>
+    </row>
+    <row r="380" spans="4:30">
+      <c r="X380" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y380" s="4"/>
+      <c r="Z380" s="4"/>
+      <c r="AA380" s="4"/>
+      <c r="AB380" s="4"/>
+      <c r="AC380" s="4"/>
+      <c r="AD380" s="4"/>
+    </row>
+    <row r="381" spans="4:30">
+      <c r="X381" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y381" s="4"/>
+      <c r="Z381" s="4"/>
+      <c r="AA381" s="4"/>
+      <c r="AB381" s="4"/>
+      <c r="AC381" s="4"/>
+      <c r="AD381" s="4"/>
+    </row>
+    <row r="382" spans="4:30">
+      <c r="X382" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y382" s="4"/>
+      <c r="Z382" s="4"/>
+      <c r="AA382" s="4"/>
+      <c r="AB382" s="4"/>
+      <c r="AC382" s="4"/>
+      <c r="AD382" s="4"/>
+    </row>
+    <row r="383" spans="4:30">
+      <c r="X383" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y383" s="4"/>
+      <c r="Z383" s="4"/>
+      <c r="AA383" s="4"/>
+      <c r="AB383" s="4"/>
+      <c r="AC383" s="4"/>
+      <c r="AD383" s="4"/>
+    </row>
+    <row r="384" spans="4:30">
+      <c r="X384" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y384" s="4"/>
+      <c r="Z384" s="4"/>
+      <c r="AA384" s="4"/>
+      <c r="AB384" s="4"/>
+      <c r="AC384" s="4"/>
+      <c r="AD384" s="4"/>
+    </row>
+    <row r="385" spans="24:30">
+      <c r="X385" s="4"/>
+      <c r="Y385" s="20"/>
+      <c r="Z385" s="4"/>
+      <c r="AA385" s="4"/>
+      <c r="AB385" s="4"/>
+      <c r="AC385" s="4"/>
+      <c r="AD385" s="4"/>
+    </row>
+    <row r="386" spans="24:30">
+      <c r="Y386" s="17"/>
+    </row>
+    <row r="387" spans="24:30">
+      <c r="Y387" s="18"/>
+    </row>
+    <row r="388" spans="24:30">
+      <c r="Y388" s="17"/>
+    </row>
+    <row r="389" spans="24:30">
+      <c r="Y389" s="18"/>
+    </row>
+    <row r="390" spans="24:30">
+      <c r="Y390" s="17"/>
+    </row>
+    <row r="391" spans="24:30">
+      <c r="Y391" s="18"/>
+    </row>
+    <row r="392" spans="24:30">
+      <c r="Y392" s="17"/>
+    </row>
+    <row r="393" spans="24:30">
+      <c r="Y393" s="19"/>
+    </row>
+    <row r="394" spans="24:30">
+      <c r="Y394" s="19"/>
+    </row>
+    <row r="402" spans="5:32" ht="19.5">
+      <c r="Y402" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z402" s="22"/>
+      <c r="AA402" s="22"/>
+    </row>
+    <row r="403" spans="5:32" ht="19.5">
+      <c r="Y403" s="22"/>
+      <c r="Z403" s="22"/>
+      <c r="AA403" s="22"/>
+    </row>
+    <row r="404" spans="5:32">
+      <c r="Y404" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z404" s="4"/>
+      <c r="AA404" s="4"/>
+      <c r="AB404" s="4"/>
+      <c r="AC404" s="4"/>
+      <c r="AD404" s="4"/>
+      <c r="AE404" s="4"/>
+      <c r="AF404" s="4"/>
+    </row>
+    <row r="405" spans="5:32">
+      <c r="Y405" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z405" s="4"/>
+      <c r="AA405" s="4"/>
+      <c r="AB405" s="4"/>
+      <c r="AC405" s="4"/>
+      <c r="AD405" s="4"/>
+      <c r="AE405" s="4"/>
+      <c r="AF405" s="4"/>
+    </row>
+    <row r="406" spans="5:32">
+      <c r="Y406" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z406" s="4"/>
+      <c r="AA406" s="4"/>
+      <c r="AB406" s="4"/>
+      <c r="AC406" s="4"/>
+      <c r="AD406" s="4"/>
+      <c r="AE406" s="4"/>
+      <c r="AF406" s="4"/>
+    </row>
+    <row r="407" spans="5:32">
+      <c r="Y407" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z407" s="4"/>
+      <c r="AA407" s="4"/>
+      <c r="AB407" s="4"/>
+      <c r="AC407" s="4"/>
+      <c r="AD407" s="4"/>
+      <c r="AE407" s="4"/>
+      <c r="AF407" s="4"/>
+    </row>
+    <row r="408" spans="5:32">
+      <c r="Y408" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z408" s="4"/>
+      <c r="AA408" s="4"/>
+      <c r="AB408" s="4"/>
+      <c r="AC408" s="4"/>
+      <c r="AD408" s="4"/>
+      <c r="AE408" s="4"/>
+      <c r="AF408" s="4"/>
+    </row>
+    <row r="409" spans="5:32">
+      <c r="Y409" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z409" s="4"/>
+      <c r="AA409" s="4"/>
+      <c r="AB409" s="4"/>
+      <c r="AC409" s="4"/>
+      <c r="AD409" s="4"/>
+      <c r="AE409" s="4"/>
+      <c r="AF409" s="4"/>
+    </row>
+    <row r="410" spans="5:32">
+      <c r="Y410" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z410" s="4"/>
+      <c r="AA410" s="4"/>
+      <c r="AB410" s="4"/>
+      <c r="AC410" s="4"/>
+      <c r="AD410" s="4"/>
+      <c r="AE410" s="4"/>
+      <c r="AF410" s="4"/>
+    </row>
+    <row r="411" spans="5:32" ht="26.25">
+      <c r="E411" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="F411" s="23"/>
+      <c r="G411" s="23"/>
+      <c r="K411" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="L411" s="22"/>
+      <c r="M411" s="22"/>
+      <c r="N411" s="22"/>
+      <c r="O411" s="22"/>
+      <c r="P411" s="22"/>
+      <c r="Q411" s="22"/>
+      <c r="R411" s="22"/>
+      <c r="S411" s="22"/>
+      <c r="T411" s="5"/>
+      <c r="U411" s="5"/>
+      <c r="Y411" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z411" s="4"/>
+      <c r="AA411" s="4"/>
+      <c r="AB411" s="4"/>
+      <c r="AC411" s="4"/>
+      <c r="AD411" s="4"/>
+      <c r="AE411" s="4"/>
+      <c r="AF411" s="4"/>
+    </row>
+    <row r="412" spans="5:32" ht="19.5">
+      <c r="K412" s="24"/>
+      <c r="L412" s="22"/>
+      <c r="M412" s="22"/>
+      <c r="N412" s="22"/>
+      <c r="O412" s="22"/>
+      <c r="P412" s="22"/>
+      <c r="Q412" s="22"/>
+      <c r="R412" s="22"/>
+      <c r="S412" s="22"/>
+      <c r="T412" s="5"/>
+      <c r="U412" s="5"/>
+      <c r="Y412" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="413" spans="5:32" ht="19.5">
+      <c r="K413" s="24"/>
+      <c r="L413" s="22"/>
+      <c r="M413" s="22"/>
+      <c r="N413" s="22"/>
+      <c r="O413" s="22"/>
+      <c r="P413" s="22"/>
+      <c r="Q413" s="22"/>
+      <c r="R413" s="22"/>
+      <c r="S413" s="22"/>
+      <c r="T413" s="5"/>
+      <c r="U413" s="5"/>
+    </row>
+    <row r="414" spans="5:32" ht="19.5">
+      <c r="K414" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="L414" s="22"/>
+      <c r="M414" s="22"/>
+      <c r="N414" s="22"/>
+      <c r="O414" s="22"/>
+      <c r="P414" s="22"/>
+      <c r="Q414" s="22"/>
+      <c r="R414" s="22"/>
+      <c r="S414" s="22"/>
+      <c r="T414" s="5"/>
+      <c r="U414" s="5"/>
+    </row>
+    <row r="419" spans="11:23">
+      <c r="K419" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="L419" s="4"/>
+      <c r="M419" s="4"/>
+      <c r="N419" s="4"/>
+      <c r="O419" s="4"/>
+      <c r="P419" s="4"/>
+      <c r="Q419" s="4"/>
+      <c r="R419" s="4"/>
+      <c r="S419" s="4"/>
+      <c r="T419" s="4"/>
+      <c r="U419" s="4"/>
+      <c r="V419" s="4"/>
+      <c r="W419" s="4"/>
+    </row>
+    <row r="420" spans="11:23">
+      <c r="K420" s="4"/>
+      <c r="L420" s="4"/>
+      <c r="M420" s="4"/>
+      <c r="N420" s="4"/>
+      <c r="O420" s="4"/>
+      <c r="P420" s="4"/>
+      <c r="Q420" s="4"/>
+      <c r="R420" s="4"/>
+      <c r="S420" s="4"/>
+      <c r="T420" s="4"/>
+      <c r="U420" s="4"/>
+      <c r="V420" s="4"/>
+      <c r="W420" s="4"/>
+    </row>
+    <row r="421" spans="11:23">
+      <c r="K421" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L421" s="4"/>
+      <c r="M421" s="4"/>
+      <c r="N421" s="4"/>
+      <c r="O421" s="4"/>
+      <c r="P421" s="4"/>
+      <c r="Q421" s="4"/>
+      <c r="R421" s="4"/>
+      <c r="S421" s="4"/>
+      <c r="T421" s="4"/>
+      <c r="U421" s="4"/>
+      <c r="V421" s="4"/>
+      <c r="W421" s="4"/>
+    </row>
+    <row r="422" spans="11:23">
+      <c r="K422" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L422" s="4"/>
+      <c r="M422" s="4"/>
+      <c r="N422" s="4"/>
+      <c r="O422" s="4"/>
+      <c r="P422" s="4"/>
+      <c r="Q422" s="4"/>
+      <c r="R422" s="4"/>
+      <c r="S422" s="4"/>
+      <c r="T422" s="4"/>
+      <c r="U422" s="4"/>
+      <c r="V422" s="4"/>
+      <c r="W422" s="4"/>
+    </row>
+    <row r="423" spans="11:23">
+      <c r="K423" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L423" s="4"/>
+      <c r="M423" s="4"/>
+      <c r="N423" s="4"/>
+      <c r="O423" s="4"/>
+      <c r="P423" s="4"/>
+      <c r="Q423" s="4"/>
+      <c r="R423" s="4"/>
+      <c r="S423" s="4"/>
+      <c r="T423" s="4"/>
+      <c r="U423" s="4"/>
+      <c r="V423" s="4"/>
+      <c r="W423" s="4"/>
+    </row>
+    <row r="424" spans="11:23">
+      <c r="K424" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L424" s="4"/>
+      <c r="M424" s="4"/>
+      <c r="N424" s="4"/>
+      <c r="O424" s="4"/>
+      <c r="P424" s="4"/>
+      <c r="Q424" s="4"/>
+      <c r="R424" s="4"/>
+      <c r="S424" s="4"/>
+      <c r="T424" s="4"/>
+      <c r="U424" s="4"/>
+      <c r="V424" s="4"/>
+      <c r="W424" s="4"/>
+    </row>
+    <row r="425" spans="11:23">
+      <c r="K425" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L425" s="4"/>
+      <c r="M425" s="4"/>
+      <c r="N425" s="4"/>
+      <c r="O425" s="4"/>
+      <c r="P425" s="4"/>
+      <c r="Q425" s="4"/>
+      <c r="R425" s="4"/>
+      <c r="S425" s="4"/>
+      <c r="T425" s="4"/>
+      <c r="U425" s="4"/>
+      <c r="V425" s="4"/>
+      <c r="W425" s="4"/>
+    </row>
+    <row r="426" spans="11:23">
+      <c r="K426" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L426" s="4"/>
+      <c r="M426" s="4"/>
+      <c r="N426" s="4"/>
+      <c r="O426" s="4"/>
+      <c r="P426" s="4"/>
+      <c r="Q426" s="4"/>
+      <c r="R426" s="4"/>
+      <c r="S426" s="4"/>
+      <c r="T426" s="4"/>
+      <c r="U426" s="4"/>
+      <c r="V426" s="4"/>
+      <c r="W426" s="4"/>
+    </row>
+    <row r="427" spans="11:23">
+      <c r="K427" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="L427" s="4"/>
+      <c r="M427" s="4"/>
+      <c r="N427" s="4"/>
+      <c r="O427" s="4"/>
+      <c r="P427" s="4"/>
+      <c r="Q427" s="4"/>
+      <c r="R427" s="4"/>
+      <c r="S427" s="4"/>
+      <c r="T427" s="4"/>
+      <c r="U427" s="4"/>
+      <c r="V427" s="4"/>
+      <c r="W427" s="4"/>
+    </row>
+    <row r="428" spans="11:23">
+      <c r="K428" s="4"/>
+      <c r="L428" s="4"/>
+      <c r="M428" s="4"/>
+      <c r="N428" s="4"/>
+      <c r="O428" s="4"/>
+      <c r="P428" s="4"/>
+      <c r="Q428" s="4"/>
+      <c r="R428" s="4"/>
+      <c r="S428" s="4"/>
+      <c r="T428" s="4"/>
+      <c r="U428" s="4"/>
+      <c r="V428" s="4"/>
+      <c r="W428" s="4"/>
+    </row>
+    <row r="429" spans="11:23">
+      <c r="K429" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L429" s="4"/>
+      <c r="M429" s="4"/>
+      <c r="N429" s="4"/>
+      <c r="O429" s="4"/>
+      <c r="P429" s="4"/>
+      <c r="Q429" s="4"/>
+      <c r="R429" s="4"/>
+      <c r="S429" s="4"/>
+      <c r="T429" s="4"/>
+      <c r="U429" s="4"/>
+      <c r="V429" s="4"/>
+      <c r="W429" s="4"/>
+    </row>
+    <row r="430" spans="11:23">
+      <c r="K430" s="4"/>
+      <c r="L430" s="4"/>
+      <c r="M430" s="4"/>
+      <c r="N430" s="4"/>
+      <c r="O430" s="4"/>
+      <c r="P430" s="4"/>
+      <c r="Q430" s="4"/>
+      <c r="R430" s="4"/>
+      <c r="S430" s="4"/>
+      <c r="T430" s="4"/>
+      <c r="U430" s="4"/>
+      <c r="V430" s="4"/>
+      <c r="W430" s="4"/>
+    </row>
+    <row r="431" spans="11:23">
+      <c r="K431" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L431" s="4"/>
+      <c r="M431" s="4"/>
+      <c r="N431" s="4"/>
+      <c r="O431" s="4"/>
+      <c r="P431" s="4"/>
+      <c r="Q431" s="4"/>
+      <c r="R431" s="4"/>
+      <c r="S431" s="4"/>
+      <c r="T431" s="4"/>
+      <c r="U431" s="4"/>
+      <c r="V431" s="4"/>
+      <c r="W431" s="4"/>
+    </row>
+    <row r="432" spans="11:23">
+      <c r="K432" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="L432" s="4"/>
+      <c r="M432" s="4"/>
+      <c r="N432" s="4"/>
+      <c r="O432" s="4"/>
+      <c r="P432" s="4"/>
+      <c r="Q432" s="4"/>
+      <c r="R432" s="4"/>
+      <c r="S432" s="4"/>
+      <c r="T432" s="4"/>
+      <c r="U432" s="4"/>
+      <c r="V432" s="4"/>
+      <c r="W432" s="4"/>
+    </row>
+    <row r="433" spans="5:25">
+      <c r="K433" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="L433" s="4"/>
+      <c r="M433" s="4"/>
+      <c r="N433" s="4"/>
+      <c r="O433" s="4"/>
+      <c r="P433" s="4"/>
+      <c r="Q433" s="4"/>
+      <c r="R433" s="4"/>
+      <c r="S433" s="4"/>
+      <c r="T433" s="4"/>
+      <c r="U433" s="4"/>
+      <c r="V433" s="4"/>
+      <c r="W433" s="4"/>
+    </row>
+    <row r="434" spans="5:25">
+      <c r="K434" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L434" s="4"/>
+      <c r="M434" s="4"/>
+      <c r="N434" s="4"/>
+      <c r="O434" s="4"/>
+      <c r="P434" s="4"/>
+      <c r="Q434" s="4"/>
+      <c r="R434" s="4"/>
+      <c r="S434" s="4"/>
+      <c r="T434" s="4"/>
+      <c r="U434" s="4"/>
+      <c r="V434" s="4"/>
+      <c r="W434" s="4"/>
+    </row>
+    <row r="444" spans="5:25" ht="26.25">
+      <c r="E444" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="F444" s="23"/>
+      <c r="G444" s="23"/>
+    </row>
+    <row r="445" spans="5:25" ht="19.5">
+      <c r="K445" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="L445" s="22"/>
+      <c r="M445" s="22"/>
+      <c r="N445" s="22"/>
+      <c r="O445" s="22"/>
+      <c r="P445" s="22"/>
+      <c r="Q445" s="22"/>
+      <c r="R445" s="22"/>
+      <c r="S445" s="22"/>
+      <c r="T445" s="4"/>
+      <c r="U445" s="4"/>
+      <c r="V445" s="4"/>
+      <c r="W445" s="4"/>
+      <c r="X445" s="4"/>
+      <c r="Y445" s="4"/>
+    </row>
+    <row r="446" spans="5:25">
+      <c r="K446" s="4"/>
+      <c r="L446" s="4"/>
+      <c r="M446" s="4"/>
+      <c r="N446" s="4"/>
+      <c r="O446" s="4"/>
+      <c r="P446" s="4"/>
+      <c r="Q446" s="4"/>
+      <c r="R446" s="4"/>
+      <c r="S446" s="4"/>
+      <c r="T446" s="4"/>
+      <c r="U446" s="4"/>
+      <c r="V446" s="4"/>
+      <c r="W446" s="4"/>
+      <c r="X446" s="4"/>
+      <c r="Y446" s="4"/>
+    </row>
+    <row r="447" spans="5:25" ht="15.75">
+      <c r="K447" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="L447" s="26"/>
+      <c r="M447" s="26"/>
+      <c r="N447" s="26"/>
+      <c r="O447" s="26"/>
+      <c r="P447" s="26"/>
+      <c r="Q447" s="26"/>
+      <c r="R447" s="26"/>
+      <c r="S447" s="26"/>
+      <c r="T447" s="26"/>
+      <c r="U447" s="26"/>
+      <c r="V447" s="26"/>
+      <c r="W447" s="26"/>
+      <c r="X447" s="5"/>
+      <c r="Y447" s="5"/>
+    </row>
+    <row r="448" spans="5:25" ht="15.75">
+      <c r="K448" s="27"/>
+      <c r="L448" s="26"/>
+      <c r="M448" s="26"/>
+      <c r="N448" s="26"/>
+      <c r="O448" s="26"/>
+      <c r="P448" s="26"/>
+      <c r="Q448" s="26"/>
+      <c r="R448" s="26"/>
+      <c r="S448" s="26"/>
+      <c r="T448" s="26"/>
+      <c r="U448" s="26"/>
+      <c r="V448" s="26"/>
+      <c r="W448" s="26"/>
+      <c r="X448" s="5"/>
+      <c r="Y448" s="5"/>
+    </row>
+    <row r="449" spans="5:25" ht="15.75">
+      <c r="K449" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="L449" s="26"/>
+      <c r="M449" s="26"/>
+      <c r="N449" s="26"/>
+      <c r="O449" s="26"/>
+      <c r="P449" s="26"/>
+      <c r="Q449" s="26"/>
+      <c r="R449" s="26"/>
+      <c r="S449" s="26"/>
+      <c r="T449" s="26"/>
+      <c r="U449" s="26"/>
+      <c r="V449" s="26"/>
+      <c r="W449" s="26"/>
+      <c r="X449" s="5"/>
+      <c r="Y449" s="5"/>
+    </row>
+    <row r="450" spans="5:25" ht="15.75">
+      <c r="K450" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="L450" s="26"/>
+      <c r="M450" s="26"/>
+      <c r="N450" s="26"/>
+      <c r="O450" s="26"/>
+      <c r="P450" s="26"/>
+      <c r="Q450" s="26"/>
+      <c r="R450" s="26"/>
+      <c r="S450" s="26"/>
+      <c r="T450" s="26"/>
+      <c r="U450" s="26"/>
+      <c r="V450" s="26"/>
+      <c r="W450" s="26"/>
+      <c r="X450" s="5"/>
+      <c r="Y450" s="5"/>
+    </row>
+    <row r="451" spans="5:25" ht="15.75">
+      <c r="K451" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="L451" s="26"/>
+      <c r="M451" s="26"/>
+      <c r="N451" s="26"/>
+      <c r="O451" s="26"/>
+      <c r="P451" s="26"/>
+      <c r="Q451" s="26"/>
+      <c r="R451" s="26"/>
+      <c r="S451" s="26"/>
+      <c r="T451" s="26"/>
+      <c r="U451" s="26"/>
+      <c r="V451" s="26"/>
+      <c r="W451" s="26"/>
+      <c r="X451" s="5"/>
+      <c r="Y451" s="5"/>
+    </row>
+    <row r="452" spans="5:25" ht="15.75">
+      <c r="K452" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="L452" s="26"/>
+      <c r="M452" s="26"/>
+      <c r="N452" s="26"/>
+      <c r="O452" s="26"/>
+      <c r="P452" s="26"/>
+      <c r="Q452" s="26"/>
+      <c r="R452" s="26"/>
+      <c r="S452" s="26"/>
+      <c r="T452" s="26"/>
+      <c r="U452" s="26"/>
+      <c r="V452" s="26"/>
+      <c r="W452" s="26"/>
+      <c r="X452" s="5"/>
+      <c r="Y452" s="5"/>
+    </row>
+    <row r="453" spans="5:25" ht="15.75">
+      <c r="K453" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="L453" s="26"/>
+      <c r="M453" s="26"/>
+      <c r="N453" s="26"/>
+      <c r="O453" s="26"/>
+      <c r="P453" s="26"/>
+      <c r="Q453" s="26"/>
+      <c r="R453" s="26"/>
+      <c r="S453" s="26"/>
+      <c r="T453" s="26"/>
+      <c r="U453" s="26"/>
+      <c r="V453" s="26"/>
+      <c r="W453" s="26"/>
+      <c r="X453" s="5"/>
+      <c r="Y453" s="5"/>
+    </row>
+    <row r="454" spans="5:25" ht="15.75">
+      <c r="K454" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="L454" s="26"/>
+      <c r="M454" s="26"/>
+      <c r="N454" s="26"/>
+      <c r="O454" s="26"/>
+      <c r="P454" s="26"/>
+      <c r="Q454" s="26"/>
+      <c r="R454" s="26"/>
+      <c r="S454" s="26"/>
+      <c r="T454" s="26"/>
+      <c r="U454" s="26"/>
+      <c r="V454" s="26"/>
+      <c r="W454" s="26"/>
+      <c r="X454" s="5"/>
+      <c r="Y454" s="5"/>
+    </row>
+    <row r="460" spans="5:25" ht="26.25">
+      <c r="E460" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F460" s="23"/>
+      <c r="G460" s="23"/>
+    </row>
+    <row r="462" spans="5:25" ht="15.75">
+      <c r="K462" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="L462" s="29"/>
+      <c r="M462" s="29"/>
+      <c r="N462" s="29"/>
+      <c r="O462" s="29"/>
+      <c r="P462" s="29"/>
+      <c r="Q462" s="29"/>
+      <c r="R462" s="29"/>
+      <c r="S462" s="29"/>
+      <c r="T462" s="29"/>
+      <c r="U462" s="29"/>
+    </row>
+    <row r="463" spans="5:25" ht="15.75">
+      <c r="K463" s="29"/>
+      <c r="L463" s="29"/>
+      <c r="M463" s="29"/>
+      <c r="N463" s="29"/>
+      <c r="O463" s="29"/>
+      <c r="P463" s="29"/>
+      <c r="Q463" s="29"/>
+      <c r="R463" s="29"/>
+      <c r="S463" s="29"/>
+      <c r="T463" s="29"/>
+      <c r="U463" s="29"/>
+    </row>
+    <row r="464" spans="5:25">
+      <c r="K464" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="L464" s="4"/>
+      <c r="M464" s="4"/>
+      <c r="N464" s="4"/>
+      <c r="O464" s="4"/>
+      <c r="P464" s="4"/>
+      <c r="Q464" s="4"/>
+      <c r="R464" s="4"/>
+      <c r="S464" s="4"/>
+      <c r="T464" s="4"/>
+      <c r="U464" s="4"/>
+    </row>
+    <row r="465" spans="11:21">
+      <c r="K465" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="L465" s="4"/>
+      <c r="M465" s="4"/>
+      <c r="N465" s="4"/>
+      <c r="O465" s="4"/>
+      <c r="P465" s="4"/>
+      <c r="Q465" s="4"/>
+      <c r="R465" s="4"/>
+      <c r="S465" s="4"/>
+      <c r="T465" s="4"/>
+      <c r="U465" s="4"/>
+    </row>
+    <row r="466" spans="11:21">
+      <c r="K466" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="L466" s="4"/>
+      <c r="M466" s="4"/>
+      <c r="N466" s="4"/>
+      <c r="O466" s="4"/>
+      <c r="P466" s="4"/>
+      <c r="Q466" s="4"/>
+      <c r="R466" s="4"/>
+      <c r="S466" s="4"/>
+      <c r="T466" s="4"/>
+      <c r="U466" s="4"/>
+    </row>
+    <row r="467" spans="11:21">
+      <c r="K467" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L467" s="4"/>
+      <c r="M467" s="4"/>
+      <c r="N467" s="4"/>
+      <c r="O467" s="4"/>
+      <c r="P467" s="4"/>
+      <c r="Q467" s="4"/>
+      <c r="R467" s="4"/>
+      <c r="S467" s="4"/>
+      <c r="T467" s="4"/>
+      <c r="U467" s="4"/>
+    </row>
+    <row r="468" spans="11:21">
+      <c r="K468" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L468" s="4"/>
+      <c r="M468" s="4"/>
+      <c r="N468" s="4"/>
+      <c r="O468" s="4"/>
+      <c r="P468" s="4"/>
+      <c r="Q468" s="4"/>
+      <c r="R468" s="4"/>
+      <c r="S468" s="4"/>
+      <c r="T468" s="4"/>
+      <c r="U468" s="4"/>
+    </row>
+    <row r="469" spans="11:21">
+      <c r="K469" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L469" s="4"/>
+      <c r="M469" s="4"/>
+      <c r="N469" s="4"/>
+      <c r="O469" s="4"/>
+      <c r="P469" s="4"/>
+      <c r="Q469" s="4"/>
+      <c r="R469" s="4"/>
+      <c r="S469" s="4"/>
+      <c r="T469" s="4"/>
+      <c r="U469" s="4"/>
+    </row>
+    <row r="470" spans="11:21">
+      <c r="K470" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="L470" s="4"/>
+      <c r="M470" s="4"/>
+      <c r="N470" s="4"/>
+      <c r="O470" s="4"/>
+      <c r="P470" s="4"/>
+      <c r="Q470" s="4"/>
+      <c r="R470" s="4"/>
+      <c r="S470" s="4"/>
+      <c r="T470" s="4"/>
+      <c r="U470" s="4"/>
+    </row>
+    <row r="471" spans="11:21">
+      <c r="K471" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L471" s="4"/>
+      <c r="M471" s="4"/>
+      <c r="N471" s="4"/>
+      <c r="O471" s="4"/>
+      <c r="P471" s="4"/>
+      <c r="Q471" s="4"/>
+      <c r="R471" s="4"/>
+      <c r="S471" s="4"/>
+      <c r="T471" s="4"/>
+      <c r="U471" s="4"/>
+    </row>
+    <row r="472" spans="11:21">
+      <c r="K472" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="L472" s="4"/>
+      <c r="M472" s="4"/>
+      <c r="N472" s="4"/>
+      <c r="O472" s="4"/>
+      <c r="P472" s="4"/>
+      <c r="Q472" s="4"/>
+      <c r="R472" s="4"/>
+      <c r="S472" s="4"/>
+      <c r="T472" s="4"/>
+      <c r="U472" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2007,6 +3573,59 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
   <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId6" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>24</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>393</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>28</xdr:col>
+                <xdr:colOff>447675</xdr:colOff>
+                <xdr:row>397</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId6" name="Control 2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId8" name="Control 1">
+          <controlPr defaultSize="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>24</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>392</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>28</xdr:col>
+                <xdr:colOff>447675</xdr:colOff>
+                <xdr:row>396</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId8" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
 </worksheet>
 </file>
 
@@ -2018,19 +3637,19 @@
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8">
       <c r="C7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:8">
       <c r="C10" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8">
       <c r="C12" s="4" t="s">
         <v>42</v>
       </c>
@@ -2040,7 +3659,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8">
       <c r="C13" s="4" t="s">
         <v>43</v>
       </c>
@@ -2050,7 +3669,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:8">
       <c r="C14" s="4" t="s">
         <v>44</v>
       </c>
@@ -2060,7 +3679,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:8">
       <c r="C15" s="4" t="s">
         <v>41</v>
       </c>
@@ -2070,7 +3689,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:8">
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>

</xml_diff>